<commit_message>
rerun lm; add permuted models brs, sdnn
</commit_message>
<xml_diff>
--- a/results/221021_femalesDBP_linreg.xlsx
+++ b/results/221021_femalesDBP_linreg.xlsx
@@ -431,19 +431,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>1.17</v>
+        <v>1.65</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.31</v>
+        <v>0.16</v>
       </c>
       <c r="E2" t="n">
-        <v>2.64</v>
+        <v>3.15</v>
       </c>
       <c r="F2" t="n">
-        <v>0.11968</v>
+        <v>0.03054</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0523</v>
+        <v>0.03152</v>
       </c>
     </row>
     <row r="3">
@@ -454,19 +454,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.16</v>
+        <v>-1.1</v>
       </c>
       <c r="D3" t="n">
         <v>-2.62</v>
       </c>
       <c r="E3" t="n">
-        <v>0.31</v>
+        <v>0.41</v>
       </c>
       <c r="F3" t="n">
-        <v>0.12022</v>
+        <v>0.15274</v>
       </c>
       <c r="G3" t="n">
-        <v>0.50563</v>
+        <v>0.52236</v>
       </c>
     </row>
     <row r="4">
@@ -477,19 +477,19 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0.23</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.18</v>
+        <v>-1.42</v>
       </c>
       <c r="E4" t="n">
-        <v>1.63</v>
+        <v>1.42</v>
       </c>
       <c r="F4" t="n">
-        <v>0.74817</v>
+        <v>0.99913</v>
       </c>
       <c r="G4" t="n">
-        <v>0.86188</v>
+        <v>0.64396</v>
       </c>
     </row>
     <row r="5">
@@ -500,19 +500,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>2.2</v>
+        <v>2.55</v>
       </c>
       <c r="D5" t="n">
-        <v>0.76</v>
+        <v>1.09</v>
       </c>
       <c r="E5" t="n">
-        <v>3.63</v>
+        <v>4.02</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00285</v>
+        <v>0.00073</v>
       </c>
       <c r="G5" t="n">
-        <v>0.96768</v>
+        <v>0.91431</v>
       </c>
     </row>
     <row r="6">
@@ -523,19 +523,19 @@
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.08</v>
+        <v>-1.79</v>
       </c>
       <c r="D6" t="n">
-        <v>-3.56</v>
+        <v>-3.33</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.6</v>
+        <v>-0.24</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00616</v>
+        <v>0.02378</v>
       </c>
       <c r="G6" t="n">
-        <v>0.06497</v>
+        <v>0.09023</v>
       </c>
     </row>
     <row r="7">
@@ -546,19 +546,19 @@
         <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.35</v>
+        <v>-0.31</v>
       </c>
       <c r="D7" t="n">
-        <v>-1.79</v>
+        <v>-1.8</v>
       </c>
       <c r="E7" t="n">
-        <v>1.09</v>
+        <v>1.19</v>
       </c>
       <c r="F7" t="n">
-        <v>0.63231</v>
+        <v>0.68721</v>
       </c>
       <c r="G7" t="n">
-        <v>0.59241</v>
+        <v>0.60731</v>
       </c>
     </row>
     <row r="8">
@@ -569,19 +569,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.73</v>
+        <v>-0.27</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.41</v>
+        <v>-2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.95</v>
+        <v>1.46</v>
       </c>
       <c r="F8" t="n">
-        <v>0.39522</v>
+        <v>0.75797</v>
       </c>
       <c r="G8" t="n">
-        <v>0.55939</v>
+        <v>0.71809</v>
       </c>
     </row>
     <row r="9">
@@ -592,19 +592,19 @@
         <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.16</v>
+        <v>-0.26</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.67</v>
+        <v>-1.78</v>
       </c>
       <c r="E9" t="n">
-        <v>1.36</v>
+        <v>1.26</v>
       </c>
       <c r="F9" t="n">
-        <v>0.83982</v>
+        <v>0.73797</v>
       </c>
       <c r="G9" t="n">
-        <v>0.97913</v>
+        <v>0.98574</v>
       </c>
     </row>
     <row r="10">
@@ -615,19 +615,19 @@
         <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>0.36</v>
+        <v>0.86</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.28</v>
+        <v>-0.78</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F10" t="n">
-        <v>0.66368</v>
+        <v>0.30416</v>
       </c>
       <c r="G10" t="n">
-        <v>0.33658</v>
+        <v>0.24896</v>
       </c>
     </row>
     <row r="11">
@@ -638,19 +638,19 @@
         <v>17</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.15</v>
+        <v>-0.79</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.61</v>
+        <v>-2.31</v>
       </c>
       <c r="E11" t="n">
-        <v>0.31</v>
+        <v>0.73</v>
       </c>
       <c r="F11" t="n">
-        <v>0.12288</v>
+        <v>0.30754</v>
       </c>
       <c r="G11" t="n">
-        <v>0.39683</v>
+        <v>0.37328</v>
       </c>
     </row>
     <row r="12">
@@ -661,19 +661,19 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.73</v>
+        <v>-0.75</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.49</v>
+        <v>-2.51</v>
       </c>
       <c r="E12" t="n">
-        <v>1.04</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.41744</v>
+        <v>0.39657</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0523</v>
+        <v>0.03152</v>
       </c>
     </row>
     <row r="13">
@@ -684,19 +684,19 @@
         <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.74</v>
+        <v>-0.75</v>
       </c>
       <c r="D13" t="n">
-        <v>-2.53</v>
+        <v>-2.54</v>
       </c>
       <c r="E13" t="n">
-        <v>1.06</v>
+        <v>1.03</v>
       </c>
       <c r="F13" t="n">
-        <v>0.42033</v>
+        <v>0.40752</v>
       </c>
       <c r="G13" t="n">
-        <v>0.50563</v>
+        <v>0.52236</v>
       </c>
     </row>
     <row r="14">
@@ -707,19 +707,19 @@
         <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.95</v>
+        <v>-0.91</v>
       </c>
       <c r="E14" t="n">
-        <v>2.32</v>
+        <v>2.33</v>
       </c>
       <c r="F14" t="n">
-        <v>0.40886</v>
+        <v>0.38752</v>
       </c>
       <c r="G14" t="n">
-        <v>0.86188</v>
+        <v>0.64396</v>
       </c>
     </row>
     <row r="15">
@@ -730,19 +730,19 @@
         <v>11</v>
       </c>
       <c r="C15" t="n">
-        <v>2.33</v>
+        <v>2.34</v>
       </c>
       <c r="D15" t="n">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="E15" t="n">
-        <v>4.27</v>
+        <v>4.24</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01881</v>
+        <v>0.01646</v>
       </c>
       <c r="G15" t="n">
-        <v>0.96768</v>
+        <v>0.91431</v>
       </c>
     </row>
     <row r="16">
@@ -753,19 +753,19 @@
         <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="D16" t="n">
-        <v>-1.52</v>
+        <v>-1.49</v>
       </c>
       <c r="E16" t="n">
-        <v>1.95</v>
+        <v>1.94</v>
       </c>
       <c r="F16" t="n">
-        <v>0.80473</v>
+        <v>0.79419</v>
       </c>
       <c r="G16" t="n">
-        <v>0.06497</v>
+        <v>0.09023</v>
       </c>
     </row>
     <row r="17">
@@ -776,19 +776,19 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.03</v>
+        <v>-0.05</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.7</v>
+        <v>-1.71</v>
       </c>
       <c r="E17" t="n">
-        <v>1.65</v>
+        <v>1.61</v>
       </c>
       <c r="F17" t="n">
-        <v>0.97271</v>
+        <v>0.95043</v>
       </c>
       <c r="G17" t="n">
-        <v>0.59241</v>
+        <v>0.60731</v>
       </c>
     </row>
     <row r="18">
@@ -799,19 +799,19 @@
         <v>14</v>
       </c>
       <c r="C18" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="D18" t="n">
-        <v>-1.15</v>
+        <v>-1.18</v>
       </c>
       <c r="E18" t="n">
-        <v>2.25</v>
+        <v>2.18</v>
       </c>
       <c r="F18" t="n">
-        <v>0.52342</v>
+        <v>0.55724</v>
       </c>
       <c r="G18" t="n">
-        <v>0.55939</v>
+        <v>0.71809</v>
       </c>
     </row>
     <row r="19">
@@ -825,16 +825,16 @@
         <v>-0.1</v>
       </c>
       <c r="D19" t="n">
-        <v>-1.87</v>
+        <v>-1.86</v>
       </c>
       <c r="E19" t="n">
-        <v>1.67</v>
+        <v>1.66</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9112</v>
+        <v>0.90869</v>
       </c>
       <c r="G19" t="n">
-        <v>0.97913</v>
+        <v>0.98574</v>
       </c>
     </row>
     <row r="20">
@@ -845,19 +845,19 @@
         <v>16</v>
       </c>
       <c r="C20" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.31</v>
+        <v>-1.27</v>
       </c>
       <c r="E20" t="n">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="F20" t="n">
-        <v>0.69392</v>
+        <v>0.67125</v>
       </c>
       <c r="G20" t="n">
-        <v>0.33658</v>
+        <v>0.24896</v>
       </c>
     </row>
     <row r="21">
@@ -868,19 +868,19 @@
         <v>17</v>
       </c>
       <c r="C21" t="n">
-        <v>0.25</v>
+        <v>0.31</v>
       </c>
       <c r="D21" t="n">
-        <v>-1.51</v>
+        <v>-1.41</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="F21" t="n">
-        <v>0.78016</v>
+        <v>0.72314</v>
       </c>
       <c r="G21" t="n">
-        <v>0.39683</v>
+        <v>0.37328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>